<commit_message>
Update Sales and Staffing Charts.xlsx
</commit_message>
<xml_diff>
--- a/data/Sales and Staffing Charts.xlsx
+++ b/data/Sales and Staffing Charts.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jake\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://culinarystaffing-my.sharepoint.com/personal/jake_golivestaffing_com/Documents/Documents/GitHub/GoLive_Staffing/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AE5846BF-940B-4D2C-884D-E857B5928A18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="8_{AE5846BF-940B-4D2C-884D-E857B5928A18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5AE54801-DBEE-4B13-8A99-298F18E97347}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A3B2B6D9-7C24-445E-A372-57A39B7AE13F}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{A3B2B6D9-7C24-445E-A372-57A39B7AE13F}"/>
   </bookViews>
   <sheets>
     <sheet name="Revenue" sheetId="1" r:id="rId1"/>
@@ -149,25 +149,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -505,7 +502,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F816EB9-28A4-4EE2-B083-40DDC67AF2B4}">
   <dimension ref="A1:F53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F45" sqref="F45"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -518,992 +517,998 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="6">
+      <c r="A2" s="3">
         <v>45662</v>
       </c>
-      <c r="B2" s="7">
+      <c r="B2" s="5">
         <v>174294.80000000002</v>
       </c>
-      <c r="C2" s="8">
+      <c r="C2" s="6">
         <v>182536.52999999997</v>
       </c>
-      <c r="D2" s="7">
+      <c r="D2" s="5">
         <v>44120.2</v>
       </c>
-      <c r="E2" s="9">
+      <c r="E2" s="7">
         <v>0.25313549228089416</v>
       </c>
-      <c r="F2" s="9">
+      <c r="F2" s="7">
         <v>-4.5151126736111102E-2</v>
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="6">
+      <c r="A3" s="3">
         <v>45669</v>
       </c>
-      <c r="B3" s="8">
+      <c r="B3" s="6">
         <v>191927.61000000004</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C3" s="6">
         <v>243076.1799999997</v>
       </c>
-      <c r="D3" s="8">
+      <c r="D3" s="6">
         <v>46136.89</v>
       </c>
-      <c r="E3" s="9">
+      <c r="E3" s="7">
         <v>0.24038693547009723</v>
       </c>
-      <c r="F3" s="9">
+      <c r="F3" s="7">
         <v>-0.21042197553046837</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="6">
+      <c r="A4" s="3">
         <v>45676</v>
       </c>
-      <c r="B4" s="7">
+      <c r="B4" s="5">
         <v>203981.36</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4" s="6">
         <v>278804.31999999972</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="6">
         <v>39897.97</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E4" s="7">
         <v>0.19559615643311723</v>
       </c>
-      <c r="F4" s="9">
+      <c r="F4" s="7">
         <v>-0.26837087746703425</v>
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="6">
+      <c r="A5" s="3">
         <v>45683</v>
       </c>
-      <c r="B5" s="8">
+      <c r="B5" s="6">
         <v>227462.55999999997</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C5" s="6">
         <v>325526.04999999946</v>
       </c>
-      <c r="D5" s="8">
+      <c r="D5" s="6">
         <v>40608.269999999997</v>
       </c>
-      <c r="E5" s="9">
+      <c r="E5" s="7">
         <v>0.17852727059785137</v>
       </c>
-      <c r="F5" s="9">
+      <c r="F5" s="7">
         <v>-0.30124621362867787</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="6">
+      <c r="A6" s="3">
         <v>45690</v>
       </c>
-      <c r="B6" s="7">
+      <c r="B6" s="5">
         <v>258094.00000000003</v>
       </c>
-      <c r="C6" s="8">
+      <c r="C6" s="6">
         <v>310656.64999999967</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D6" s="6">
         <v>29584.42</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6" s="7">
         <v>0.11462653141878539</v>
       </c>
-      <c r="F6" s="9">
+      <c r="F6" s="7">
         <v>-0.16919853478108293</v>
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="6">
+      <c r="A7" s="3">
         <v>45697</v>
       </c>
-      <c r="B7" s="8">
+      <c r="B7" s="6">
         <v>211035.74</v>
       </c>
-      <c r="C7" s="8">
+      <c r="C7" s="6">
         <v>307344.53999999957</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="6">
         <v>35424.82</v>
       </c>
-      <c r="E7" s="9">
+      <c r="E7" s="7">
         <v>0.16786170911145193</v>
       </c>
-      <c r="F7" s="9">
+      <c r="F7" s="7">
         <v>-0.31335777105394391</v>
       </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="6">
+      <c r="A8" s="3">
         <v>45704</v>
       </c>
-      <c r="B8" s="7">
+      <c r="B8" s="5">
         <v>210595.28999999989</v>
       </c>
-      <c r="C8" s="8">
+      <c r="C8" s="6">
         <v>327003.24000000022</v>
       </c>
-      <c r="D8" s="8">
+      <c r="D8" s="6">
         <v>39715.01</v>
       </c>
-      <c r="E8" s="9">
+      <c r="E8" s="7">
         <v>0.18858451202778573</v>
       </c>
-      <c r="F8" s="9">
+      <c r="F8" s="7">
         <v>-0.35598408749711552</v>
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="6">
+      <c r="A9" s="3">
         <v>45711</v>
       </c>
-      <c r="B9" s="8">
+      <c r="B9" s="6">
         <v>183039.22999999998</v>
       </c>
-      <c r="C9" s="8">
+      <c r="C9" s="6">
         <v>282217.79999999958</v>
       </c>
-      <c r="D9" s="8">
+      <c r="D9" s="6">
         <v>38615.360000000001</v>
       </c>
-      <c r="E9" s="9">
+      <c r="E9" s="7">
         <v>0.21096767070097489</v>
       </c>
-      <c r="F9" s="9">
+      <c r="F9" s="7">
         <v>-0.35142563651194125</v>
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="6">
+      <c r="A10" s="3">
         <v>45718</v>
       </c>
-      <c r="B10" s="7">
+      <c r="B10" s="5">
         <v>278609.68999999994</v>
       </c>
-      <c r="C10" s="8">
+      <c r="C10" s="6">
         <v>406848.86999999994</v>
       </c>
-      <c r="D10" s="8">
+      <c r="D10" s="6">
         <v>34311.769999999997</v>
       </c>
-      <c r="E10" s="9">
+      <c r="E10" s="7">
         <v>0.12315354142923027</v>
       </c>
-      <c r="F10" s="9">
+      <c r="F10" s="7">
         <v>-0.31520102292529417</v>
       </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="6">
+      <c r="A11" s="3">
         <v>45725</v>
       </c>
-      <c r="B11" s="7">
+      <c r="B11" s="5">
         <v>226781.59</v>
       </c>
-      <c r="C11" s="8">
+      <c r="C11" s="6">
         <v>492946.42999999959</v>
       </c>
-      <c r="D11" s="8">
+      <c r="D11" s="6">
         <v>36215.15</v>
       </c>
-      <c r="E11" s="9">
+      <c r="E11" s="7">
         <v>0.15969175452028536</v>
       </c>
-      <c r="F11" s="9">
+      <c r="F11" s="7">
         <v>-0.53994678488694969</v>
       </c>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="6">
+      <c r="A12" s="3">
         <v>45732</v>
       </c>
-      <c r="B12" s="7">
+      <c r="B12" s="5">
         <v>204801.6999999999</v>
       </c>
-      <c r="C12" s="8">
+      <c r="C12" s="6">
         <v>468207.41000000003</v>
       </c>
-      <c r="D12" s="8">
+      <c r="D12" s="6">
         <v>40701.64</v>
       </c>
-      <c r="E12" s="9">
+      <c r="E12" s="7">
         <v>0.19873682689157376</v>
       </c>
-      <c r="F12" s="9">
+      <c r="F12" s="7">
         <v>-0.56258338585457268</v>
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="6">
+      <c r="A13" s="3">
         <v>45739</v>
       </c>
-      <c r="B13" s="7">
+      <c r="B13" s="5">
         <v>273834.16000000009</v>
       </c>
-      <c r="C13" s="8">
+      <c r="C13" s="6">
         <v>375603.12999999931</v>
       </c>
-      <c r="D13" s="8">
+      <c r="D13" s="6">
         <v>38585.089999999997</v>
       </c>
-      <c r="E13" s="9">
+      <c r="E13" s="7">
         <v>0.14090678095092293</v>
       </c>
-      <c r="F13" s="9">
+      <c r="F13" s="7">
         <v>-0.27094814145984192</v>
       </c>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="6">
+      <c r="A14" s="3">
         <v>45746</v>
       </c>
-      <c r="B14" s="7">
+      <c r="B14" s="5">
         <v>248135.13</v>
       </c>
-      <c r="C14" s="8">
+      <c r="C14" s="6">
         <v>340411.14000000025</v>
       </c>
-      <c r="D14" s="8">
+      <c r="D14" s="6">
         <v>44522.61</v>
       </c>
-      <c r="E14" s="9">
+      <c r="E14" s="7">
         <v>0.17942888618794123</v>
       </c>
-      <c r="F14" s="9">
+      <c r="F14" s="7">
         <v>-0.27107223929275692</v>
       </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="6">
+      <c r="A15" s="3">
         <v>45753</v>
       </c>
-      <c r="B15" s="7">
+      <c r="B15" s="5">
         <v>242723.59</v>
       </c>
-      <c r="C15" s="8">
+      <c r="C15" s="6">
         <v>273530.54999999987</v>
       </c>
-      <c r="D15" s="8">
+      <c r="D15" s="6">
         <v>32490.55</v>
       </c>
-      <c r="E15" s="9">
+      <c r="E15" s="7">
         <v>0.13385822943703166</v>
       </c>
-      <c r="F15" s="9">
+      <c r="F15" s="7">
         <v>-0.11262712702475053</v>
       </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="6">
+      <c r="A16" s="3">
         <v>45760</v>
       </c>
-      <c r="B16" s="7">
+      <c r="B16" s="5">
         <v>226637.23000000004</v>
       </c>
-      <c r="C16" s="8">
+      <c r="C16" s="6">
         <v>390090.2900000001</v>
       </c>
-      <c r="D16" s="8">
+      <c r="D16" s="6">
         <v>33837.99</v>
       </c>
-      <c r="E16" s="9">
+      <c r="E16" s="7">
         <v>0.14930463984227124</v>
       </c>
-      <c r="F16" s="9">
+      <c r="F16" s="7">
         <v>-0.41901340328158387</v>
       </c>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="6">
+      <c r="A17" s="3">
         <v>45767</v>
       </c>
-      <c r="B17" s="7">
+      <c r="B17" s="5">
         <v>200605.52000000002</v>
       </c>
-      <c r="C17" s="8">
+      <c r="C17" s="6">
         <v>313611.45000000007</v>
       </c>
-      <c r="D17" s="8">
+      <c r="D17" s="6">
         <v>17636.990000000002</v>
       </c>
-      <c r="E17" s="9">
+      <c r="E17" s="7">
         <v>8.7918767140605106E-2</v>
       </c>
-      <c r="F17" s="9">
+      <c r="F17" s="7">
         <v>-0.36033738564073481</v>
       </c>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" s="6">
+      <c r="A18" s="3">
         <v>45774</v>
       </c>
-      <c r="B18" s="7">
+      <c r="B18" s="5">
         <v>265410</v>
       </c>
-      <c r="C18" s="8">
+      <c r="C18" s="6">
         <v>352412.92999999953</v>
       </c>
-      <c r="D18" s="8">
+      <c r="D18" s="6">
         <v>19405.37</v>
       </c>
-      <c r="E18" s="9">
+      <c r="E18" s="7">
         <v>7.3114690478881722E-2</v>
       </c>
-      <c r="F18" s="9">
+      <c r="F18" s="7">
         <v>-0.24687780326334685</v>
       </c>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="6">
+      <c r="A19" s="3">
         <v>45781</v>
       </c>
-      <c r="B19" s="7">
+      <c r="B19" s="5">
         <v>259075.19000000006</v>
       </c>
-      <c r="C19" s="8">
+      <c r="C19" s="6">
         <v>364950.25999999949</v>
       </c>
-      <c r="D19" s="8">
+      <c r="D19" s="6">
         <v>26001.22</v>
       </c>
-      <c r="E19" s="9">
+      <c r="E19" s="7">
         <v>0.10036167492533729</v>
       </c>
-      <c r="F19" s="9">
+      <c r="F19" s="7">
         <v>-0.29010821913101137</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="15.75">
-      <c r="A20" s="6">
+      <c r="A20" s="3">
         <v>45788</v>
       </c>
-      <c r="B20" s="10">
+      <c r="B20" s="8">
         <v>261020.14</v>
       </c>
-      <c r="C20" s="8">
+      <c r="C20" s="6">
         <v>425529.93000000058</v>
       </c>
-      <c r="D20" s="8">
+      <c r="D20" s="6">
         <v>24131.13</v>
       </c>
-      <c r="E20" s="9">
+      <c r="E20" s="7">
         <v>9.2449302954170504E-2</v>
       </c>
-      <c r="F20" s="9">
+      <c r="F20" s="7">
         <v>-0.38659980979481356</v>
       </c>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="6">
+      <c r="A21" s="3">
         <v>45795</v>
       </c>
-      <c r="B21" s="8">
+      <c r="B21" s="6">
         <v>238589.45000000004</v>
       </c>
-      <c r="C21" s="8">
+      <c r="C21" s="6">
         <v>336398.62999999977</v>
       </c>
-      <c r="D21" s="8">
+      <c r="D21" s="6">
         <v>28214.74</v>
       </c>
-      <c r="E21" s="9">
+      <c r="E21" s="7">
         <v>0.11825644428117001</v>
       </c>
-      <c r="F21" s="9">
+      <c r="F21" s="7">
         <v>-0.29075380003777007</v>
       </c>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" s="6">
+      <c r="A22" s="3">
         <v>45802</v>
       </c>
-      <c r="B22" s="8">
+      <c r="B22" s="6">
         <v>239882.77</v>
       </c>
-      <c r="C22" s="8">
+      <c r="C22" s="6">
         <v>308474.0399999998</v>
       </c>
-      <c r="D22" s="8">
+      <c r="D22" s="6">
         <v>21013.759999999998</v>
       </c>
-      <c r="E22" s="9">
+      <c r="E22" s="7">
         <v>8.7600122343092834E-2</v>
       </c>
-      <c r="F22" s="9">
+      <c r="F22" s="7">
         <v>-0.22235670139373753</v>
       </c>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="6">
+      <c r="A23" s="3">
         <v>45809</v>
       </c>
-      <c r="B23" s="8">
+      <c r="B23" s="6">
         <v>185195.06000000006</v>
       </c>
-      <c r="C23" s="8">
+      <c r="C23" s="6">
         <v>265417.39000000007</v>
       </c>
-      <c r="D23" s="8">
+      <c r="D23" s="6">
         <v>24408.86</v>
       </c>
-      <c r="E23" s="9">
+      <c r="E23" s="7">
         <v>0.13180081585329539</v>
       </c>
-      <c r="F23" s="9">
+      <c r="F23" s="7">
         <v>-0.30224971317817573</v>
       </c>
     </row>
     <row r="24" spans="1:6">
-      <c r="A24" s="6">
+      <c r="A24" s="3">
         <v>45816</v>
       </c>
-      <c r="B24" s="8">
+      <c r="B24" s="6">
         <v>230346.97000000003</v>
       </c>
-      <c r="C24" s="8">
+      <c r="C24" s="6">
         <v>370097.93999999989</v>
       </c>
-      <c r="D24" s="8">
+      <c r="D24" s="6">
         <v>27792.94</v>
       </c>
-      <c r="E24" s="9">
+      <c r="E24" s="7">
         <v>0.120656850836805</v>
       </c>
-      <c r="F24" s="9">
+      <c r="F24" s="7">
         <v>-0.37760537116202242</v>
       </c>
     </row>
     <row r="25" spans="1:6">
-      <c r="A25" s="6">
+      <c r="A25" s="3">
         <v>45823</v>
       </c>
-      <c r="B25" s="8">
+      <c r="B25" s="6">
         <v>211413.24000000002</v>
       </c>
-      <c r="C25" s="8">
+      <c r="C25" s="6">
         <v>322732.31999999989</v>
       </c>
-      <c r="D25" s="8">
+      <c r="D25" s="6">
         <v>15232.25</v>
       </c>
-      <c r="E25" s="9">
+      <c r="E25" s="7">
         <v>7.2049650248962635E-2</v>
       </c>
-      <c r="F25" s="9">
+      <c r="F25" s="7">
         <v>-0.34492696609995521</v>
       </c>
     </row>
     <row r="26" spans="1:6">
-      <c r="A26" s="6">
+      <c r="A26" s="3">
         <v>45830</v>
       </c>
-      <c r="B26" s="8">
+      <c r="B26" s="6">
         <v>194498.18000000005</v>
       </c>
-      <c r="C26" s="8">
+      <c r="C26" s="6">
         <v>317908.49999999983</v>
       </c>
-      <c r="D26" s="8">
+      <c r="D26" s="6">
         <v>19490.28</v>
       </c>
-      <c r="E26" s="9">
+      <c r="E26" s="7">
         <v>0.10020803279495979</v>
       </c>
-      <c r="F26" s="9">
+      <c r="F26" s="7">
         <v>-0.38819446475951369</v>
       </c>
     </row>
     <row r="27" spans="1:6">
-      <c r="A27" s="6">
+      <c r="A27" s="3">
         <v>45837</v>
       </c>
-      <c r="B27" s="8">
+      <c r="B27" s="6">
         <v>216449.77000000005</v>
       </c>
-      <c r="C27" s="8">
+      <c r="C27" s="6">
         <v>331006.54999999987</v>
       </c>
-      <c r="D27" s="8">
+      <c r="D27" s="6">
         <v>37972.67</v>
       </c>
-      <c r="E27" s="9">
+      <c r="E27" s="7">
         <v>0.17543409725036893</v>
       </c>
-      <c r="F27" s="9">
+      <c r="F27" s="7">
         <v>-0.34608614240413027</v>
       </c>
     </row>
     <row r="28" spans="1:6">
-      <c r="A28" s="6">
+      <c r="A28" s="3">
         <v>45844</v>
       </c>
-      <c r="B28" s="8">
+      <c r="B28" s="6">
         <v>150571.54999999999</v>
       </c>
-      <c r="C28" s="8">
+      <c r="C28" s="6">
         <v>241221.7500000002</v>
       </c>
-      <c r="D28" s="8">
+      <c r="D28" s="6">
         <v>17824.099999999999</v>
       </c>
-      <c r="E28" s="9">
+      <c r="E28" s="7">
         <v>0.11837628024683282</v>
       </c>
-      <c r="F28" s="9">
+      <c r="F28" s="7">
         <v>-0.375796129494957</v>
       </c>
     </row>
     <row r="29" spans="1:6">
-      <c r="A29" s="6">
+      <c r="A29" s="3">
         <v>45851</v>
       </c>
-      <c r="B29" s="8">
+      <c r="B29" s="6">
         <v>169364.16000000006</v>
       </c>
-      <c r="C29" s="8">
+      <c r="C29" s="6">
         <v>258857.03999999975</v>
       </c>
-      <c r="D29" s="11">
+      <c r="D29" s="9">
         <v>24135.43</v>
       </c>
-      <c r="E29" s="9">
+      <c r="E29" s="7">
         <v>0.1425061240819781</v>
       </c>
-      <c r="F29" s="9">
+      <c r="F29" s="7">
         <v>-0.34572318373106548</v>
       </c>
     </row>
     <row r="30" spans="1:6">
-      <c r="A30" s="6">
+      <c r="A30" s="3">
         <v>45858</v>
       </c>
-      <c r="B30" s="8">
+      <c r="B30" s="6">
         <v>197762.71000000005</v>
       </c>
-      <c r="C30" s="8">
+      <c r="C30" s="6">
         <v>307494.14999999956</v>
       </c>
-      <c r="D30" s="8">
+      <c r="D30" s="6">
         <v>31360.51</v>
       </c>
-      <c r="E30" s="9">
+      <c r="E30" s="7">
         <v>0.15857645761427921</v>
       </c>
-      <c r="F30" s="9">
+      <c r="F30" s="7">
         <v>-0.35685700036894907</v>
       </c>
     </row>
     <row r="31" spans="1:6">
-      <c r="A31" s="6">
+      <c r="A31" s="3">
         <v>45865</v>
       </c>
-      <c r="B31" s="8">
+      <c r="B31" s="6">
         <v>185317.71000000005</v>
       </c>
-      <c r="C31" s="8">
+      <c r="C31" s="6">
         <v>291026.70999999985</v>
       </c>
-      <c r="D31" s="8">
+      <c r="D31" s="6">
         <v>34519.42</v>
       </c>
-      <c r="E31" s="9">
+      <c r="E31" s="7">
         <v>0.18627156573432721</v>
       </c>
-      <c r="F31" s="9">
+      <c r="F31" s="7">
         <v>-0.36322782881337545</v>
       </c>
     </row>
     <row r="32" spans="1:6">
-      <c r="A32" s="6">
+      <c r="A32" s="3">
         <v>45872</v>
       </c>
-      <c r="B32" s="8">
+      <c r="B32" s="6">
         <v>180767.56999999998</v>
       </c>
-      <c r="C32" s="8">
+      <c r="C32" s="6">
         <v>293420.3499999998</v>
       </c>
-      <c r="D32" s="8">
+      <c r="D32" s="6">
         <v>23957.25</v>
       </c>
-      <c r="E32" s="9">
+      <c r="E32" s="7">
         <v>0.13253068567553353</v>
       </c>
-      <c r="F32" s="9">
+      <c r="F32" s="7">
         <v>-0.38392967631590613</v>
       </c>
     </row>
     <row r="33" spans="1:6">
-      <c r="A33" s="6">
+      <c r="A33" s="3">
         <v>45879</v>
       </c>
-      <c r="B33" s="8">
+      <c r="B33" s="6">
         <v>211095.77</v>
       </c>
-      <c r="C33" s="8">
+      <c r="C33" s="6">
         <v>289832.15999999968</v>
       </c>
-      <c r="D33" s="8">
+      <c r="D33" s="6">
         <v>45357.899999999994</v>
       </c>
-      <c r="E33" s="9">
+      <c r="E33" s="7">
         <v>0.2148688247045405</v>
       </c>
-      <c r="F33" s="9">
+      <c r="F33" s="7">
         <v>-0.27166201983934346</v>
       </c>
     </row>
     <row r="34" spans="1:6">
-      <c r="A34" s="6">
+      <c r="A34" s="3">
         <v>45886</v>
       </c>
-      <c r="B34" s="8">
+      <c r="B34" s="6">
         <v>243840.95000000004</v>
       </c>
-      <c r="C34" s="8">
+      <c r="C34" s="6">
         <v>337646.1199999997</v>
       </c>
-      <c r="D34" s="8">
+      <c r="D34" s="6">
         <v>52670.850000000006</v>
       </c>
-      <c r="E34" s="9">
+      <c r="E34" s="7">
         <v>0.21600494092563205</v>
       </c>
-      <c r="F34" s="9">
+      <c r="F34" s="7">
         <v>-0.27782096237326748</v>
       </c>
     </row>
     <row r="35" spans="1:6">
-      <c r="A35" s="6">
+      <c r="A35" s="3">
         <v>45893</v>
       </c>
-      <c r="B35" s="8">
+      <c r="B35" s="6">
         <v>216233.39000000004</v>
       </c>
-      <c r="C35" s="8">
+      <c r="C35" s="6">
         <v>377961.64999999956</v>
       </c>
-      <c r="D35" s="8">
+      <c r="D35" s="6">
         <v>35063.42</v>
       </c>
-      <c r="E35" s="9">
+      <c r="E35" s="7">
         <v>0.16215543769627805</v>
       </c>
-      <c r="F35" s="9">
+      <c r="F35" s="7">
         <v>-0.42789595187765661</v>
       </c>
     </row>
     <row r="36" spans="1:6">
-      <c r="A36" s="6">
+      <c r="A36" s="3">
         <v>45900</v>
       </c>
-      <c r="B36" s="8">
+      <c r="B36" s="6">
         <v>202533.55</v>
       </c>
-      <c r="C36" s="8">
+      <c r="C36" s="6">
         <v>336254.38999999972</v>
       </c>
-      <c r="D36" s="8">
+      <c r="D36" s="6">
         <v>36863.040000000001</v>
       </c>
-      <c r="E36" s="9">
+      <c r="E36" s="7">
         <v>0.18200954854146389</v>
       </c>
-      <c r="F36" s="9">
+      <c r="F36" s="7">
         <v>-0.39767760355485571</v>
       </c>
     </row>
     <row r="37" spans="1:6">
-      <c r="A37" s="6">
+      <c r="A37" s="3">
         <v>45907</v>
       </c>
-      <c r="B37" s="8">
+      <c r="B37" s="6">
         <v>236164.89</v>
       </c>
-      <c r="C37" s="8">
+      <c r="C37" s="6">
         <v>307653.78999999957</v>
       </c>
-      <c r="D37" s="8">
+      <c r="D37" s="6">
         <v>61066.96</v>
       </c>
-      <c r="E37" s="9">
+      <c r="E37" s="7">
         <v>0.25857764039354025</v>
       </c>
-      <c r="F37" s="9">
+      <c r="F37" s="7">
         <v>-0.23236801340883739</v>
       </c>
     </row>
     <row r="38" spans="1:6">
-      <c r="A38" s="6">
+      <c r="A38" s="3">
         <v>45914</v>
       </c>
-      <c r="B38" s="8">
+      <c r="B38" s="6">
         <v>273744.57</v>
       </c>
-      <c r="C38" s="8">
+      <c r="C38" s="6">
         <v>478029.9800000001</v>
       </c>
-      <c r="D38" s="8">
+      <c r="D38" s="6">
         <v>45558.13</v>
       </c>
-      <c r="E38" s="9">
+      <c r="E38" s="7">
         <v>0.16642569385029263</v>
       </c>
-      <c r="F38" s="9">
+      <c r="F38" s="7">
         <v>-0.42734853157117891</v>
       </c>
     </row>
     <row r="39" spans="1:6">
-      <c r="A39" s="6">
+      <c r="A39" s="3">
         <v>45921</v>
       </c>
-      <c r="B39" s="8">
+      <c r="B39" s="6">
         <v>324354.64</v>
       </c>
-      <c r="C39" s="8">
+      <c r="C39" s="6">
         <v>358026.49</v>
       </c>
-      <c r="D39" s="8">
+      <c r="D39" s="6">
         <v>85075.85</v>
       </c>
-      <c r="E39" s="9">
+      <c r="E39" s="7">
         <v>0.26229268679492301</v>
       </c>
-      <c r="F39" s="9">
+      <c r="F39" s="7">
         <v>-9.4048487864682784E-2</v>
       </c>
     </row>
     <row r="40" spans="1:6">
-      <c r="A40" s="6">
+      <c r="A40" s="3">
         <v>45928</v>
       </c>
-      <c r="B40" s="8">
+      <c r="B40" s="6">
         <v>241214.18999999997</v>
       </c>
-      <c r="C40" s="8">
+      <c r="C40" s="6">
         <v>377543.97999999917</v>
       </c>
-      <c r="D40" s="8">
+      <c r="D40" s="6">
         <v>42243.31</v>
       </c>
-      <c r="E40" s="9">
+      <c r="E40" s="7">
         <v>0.17512779824437361</v>
       </c>
-      <c r="F40" s="9">
+      <c r="F40" s="7">
         <v>-0.36109644762445825</v>
       </c>
     </row>
     <row r="41" spans="1:6">
-      <c r="A41" s="6">
+      <c r="A41" s="3">
         <v>45935</v>
       </c>
-      <c r="B41" s="8">
+      <c r="B41" s="6">
         <v>247082.19999999998</v>
       </c>
-      <c r="C41" s="8">
+      <c r="C41" s="6">
         <v>357141.31999999983</v>
       </c>
-      <c r="D41" s="8">
+      <c r="D41" s="6">
         <v>66246.09</v>
       </c>
-      <c r="E41" s="9">
+      <c r="E41" s="7">
         <v>0.26811356706391637</v>
       </c>
-      <c r="F41" s="9">
+      <c r="F41" s="7">
         <v>-0.30816686235017532</v>
       </c>
     </row>
     <row r="42" spans="1:6">
-      <c r="A42" s="6">
+      <c r="A42" s="3">
         <v>45942</v>
       </c>
-      <c r="B42" s="8">
+      <c r="B42" s="6">
         <v>250229.77999999997</v>
       </c>
-      <c r="C42" s="8">
+      <c r="C42" s="6">
         <v>343271.64999999973</v>
       </c>
-      <c r="D42" s="8">
+      <c r="D42" s="6">
         <v>27464.48</v>
       </c>
-      <c r="E42" s="9">
+      <c r="E42" s="7">
         <v>0.10975704010929475</v>
       </c>
-      <c r="F42" s="9">
+      <c r="F42" s="7">
         <v>-0.27104443375967646</v>
       </c>
     </row>
     <row r="43" spans="1:6">
-      <c r="A43" s="6">
+      <c r="A43" s="3">
         <v>45949</v>
       </c>
-      <c r="B43" s="8">
+      <c r="B43" s="6">
         <v>291481.51000000007</v>
       </c>
-      <c r="C43" s="8">
+      <c r="C43" s="6">
         <v>395964.53000000026</v>
       </c>
-      <c r="D43" s="8">
+      <c r="D43" s="6">
         <v>56897.53</v>
       </c>
-      <c r="E43" s="9">
+      <c r="E43" s="7">
         <v>0.19520116387485431</v>
       </c>
-      <c r="F43" s="9">
+      <c r="F43" s="7">
         <v>-0.26386964509169575</v>
       </c>
     </row>
     <row r="44" spans="1:6">
-      <c r="A44" s="6">
+      <c r="A44" s="3">
         <v>45956</v>
       </c>
-      <c r="B44" s="8">
+      <c r="B44" s="6">
         <v>240407.28999999995</v>
       </c>
-      <c r="C44" s="8">
+      <c r="C44" s="6">
         <v>417034.32999999961</v>
       </c>
-      <c r="D44" s="8">
+      <c r="D44" s="6">
         <v>44556.4</v>
       </c>
-      <c r="E44" s="9">
+      <c r="E44" s="7">
         <v>0.18533714181462638</v>
       </c>
-      <c r="F44" s="9">
+      <c r="F44" s="7">
         <v>-0.42353117547900632</v>
       </c>
     </row>
     <row r="45" spans="1:6">
-      <c r="A45" s="6">
+      <c r="A45" s="3">
         <v>45963</v>
       </c>
-      <c r="B45" s="8"/>
-      <c r="C45" s="8">
+      <c r="B45" s="6">
+        <v>250310.42</v>
+      </c>
+      <c r="C45" s="6">
         <v>389381.13999999932</v>
       </c>
-      <c r="D45" s="8"/>
-      <c r="E45" s="9"/>
-      <c r="F45" s="9"/>
+      <c r="D45" s="6">
+        <v>54508.77</v>
+      </c>
+      <c r="E45" s="7">
+        <v>0.21779999999999999</v>
+      </c>
+      <c r="F45" s="7"/>
     </row>
     <row r="46" spans="1:6">
-      <c r="A46" s="6">
+      <c r="A46" s="3">
         <v>45970</v>
       </c>
-      <c r="B46" s="8"/>
-      <c r="C46" s="8">
+      <c r="B46" s="6"/>
+      <c r="C46" s="6">
         <v>394153.5100000003</v>
       </c>
-      <c r="D46" s="8"/>
-      <c r="E46" s="9"/>
-      <c r="F46" s="9"/>
+      <c r="D46" s="6"/>
+      <c r="E46" s="7"/>
+      <c r="F46" s="7"/>
     </row>
     <row r="47" spans="1:6">
-      <c r="A47" s="6">
+      <c r="A47" s="3">
         <v>45977</v>
       </c>
-      <c r="B47" s="8"/>
-      <c r="C47" s="8">
+      <c r="B47" s="6"/>
+      <c r="C47" s="6">
         <v>358939.24000000005</v>
       </c>
-      <c r="D47" s="8"/>
-      <c r="E47" s="9"/>
-      <c r="F47" s="9"/>
+      <c r="D47" s="6"/>
+      <c r="E47" s="7"/>
+      <c r="F47" s="7"/>
     </row>
     <row r="48" spans="1:6">
-      <c r="A48" s="6">
+      <c r="A48" s="3">
         <v>45984</v>
       </c>
-      <c r="B48" s="8"/>
-      <c r="C48" s="8">
+      <c r="B48" s="6"/>
+      <c r="C48" s="6">
         <v>527012.11999999965</v>
       </c>
-      <c r="D48" s="8"/>
-      <c r="E48" s="9"/>
-      <c r="F48" s="9"/>
+      <c r="D48" s="6"/>
+      <c r="E48" s="7"/>
+      <c r="F48" s="7"/>
     </row>
     <row r="49" spans="1:6">
-      <c r="A49" s="6">
+      <c r="A49" s="3">
         <v>45991</v>
       </c>
-      <c r="B49" s="8"/>
-      <c r="C49" s="8">
+      <c r="B49" s="6"/>
+      <c r="C49" s="6">
         <v>233700.89000000019</v>
       </c>
-      <c r="D49" s="8"/>
-      <c r="E49" s="9"/>
-      <c r="F49" s="9"/>
+      <c r="D49" s="6"/>
+      <c r="E49" s="7"/>
+      <c r="F49" s="7"/>
     </row>
     <row r="50" spans="1:6">
-      <c r="A50" s="6">
+      <c r="A50" s="3">
         <v>45998</v>
       </c>
-      <c r="B50" s="8"/>
-      <c r="C50" s="8">
+      <c r="B50" s="6"/>
+      <c r="C50" s="6">
         <v>434505.2599999996</v>
       </c>
-      <c r="D50" s="8"/>
-      <c r="E50" s="9"/>
-      <c r="F50" s="9"/>
+      <c r="D50" s="6"/>
+      <c r="E50" s="7"/>
+      <c r="F50" s="7"/>
     </row>
     <row r="51" spans="1:6">
-      <c r="A51" s="6">
+      <c r="A51" s="3">
         <v>46005</v>
       </c>
-      <c r="B51" s="8"/>
-      <c r="C51" s="8">
+      <c r="B51" s="6"/>
+      <c r="C51" s="6">
         <v>445049.27999999956</v>
       </c>
-      <c r="D51" s="8"/>
-      <c r="E51" s="9"/>
-      <c r="F51" s="9"/>
+      <c r="D51" s="6"/>
+      <c r="E51" s="7"/>
+      <c r="F51" s="7"/>
     </row>
     <row r="52" spans="1:6">
-      <c r="A52" s="6">
+      <c r="A52" s="3">
         <v>46012</v>
       </c>
-      <c r="B52" s="8"/>
-      <c r="C52" s="8">
+      <c r="B52" s="6"/>
+      <c r="C52" s="6">
         <v>245005.63000000009</v>
       </c>
-      <c r="D52" s="8"/>
-      <c r="E52" s="9"/>
-      <c r="F52" s="9"/>
+      <c r="D52" s="6"/>
+      <c r="E52" s="7"/>
+      <c r="F52" s="7"/>
     </row>
     <row r="53" spans="1:6">
-      <c r="A53" s="6">
+      <c r="A53" s="3">
         <v>46019</v>
       </c>
-      <c r="B53" s="8"/>
-      <c r="C53" s="8">
+      <c r="B53" s="6"/>
+      <c r="C53" s="6">
         <v>130961.07000000005</v>
       </c>
-      <c r="D53" s="8"/>
-      <c r="E53" s="9"/>
-      <c r="F53" s="9"/>
+      <c r="D53" s="6"/>
+      <c r="E53" s="7"/>
+      <c r="F53" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1514,13 +1519,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AC1FE54-5241-4EDC-8539-E8BDF3481B66}">
   <dimension ref="A1:G53"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="25.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.28515625" style="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1548,13 +1555,13 @@
       <c r="A2" s="3">
         <v>45662</v>
       </c>
-      <c r="B2" s="12">
+      <c r="B2" s="10">
         <v>624</v>
       </c>
       <c r="C2">
         <v>615</v>
       </c>
-      <c r="E2" s="15">
+      <c r="E2" s="3">
         <v>45662</v>
       </c>
       <c r="F2">
@@ -1568,13 +1575,13 @@
       <c r="A3" s="3">
         <v>45669</v>
       </c>
-      <c r="B3" s="12">
+      <c r="B3" s="10">
         <v>879</v>
       </c>
       <c r="C3">
         <v>686</v>
       </c>
-      <c r="E3" s="15">
+      <c r="E3" s="3">
         <v>45669</v>
       </c>
       <c r="F3">
@@ -1588,13 +1595,13 @@
       <c r="A4" s="3">
         <v>45676</v>
       </c>
-      <c r="B4" s="12">
+      <c r="B4" s="10">
         <v>1002</v>
       </c>
       <c r="C4">
         <v>733</v>
       </c>
-      <c r="E4" s="15">
+      <c r="E4" s="3">
         <v>45676</v>
       </c>
       <c r="F4">
@@ -1608,13 +1615,13 @@
       <c r="A5" s="3">
         <v>45683</v>
       </c>
-      <c r="B5" s="12">
+      <c r="B5" s="10">
         <v>1191</v>
       </c>
       <c r="C5">
         <v>845</v>
       </c>
-      <c r="E5" s="15">
+      <c r="E5" s="3">
         <v>45683</v>
       </c>
       <c r="F5">
@@ -1628,13 +1635,13 @@
       <c r="A6" s="3">
         <v>45690</v>
       </c>
-      <c r="B6" s="12">
+      <c r="B6" s="10">
         <v>1128</v>
       </c>
       <c r="C6">
         <v>1038</v>
       </c>
-      <c r="E6" s="15">
+      <c r="E6" s="3">
         <v>45690</v>
       </c>
       <c r="F6">
@@ -1648,13 +1655,13 @@
       <c r="A7" s="3">
         <v>45697</v>
       </c>
-      <c r="B7" s="12">
+      <c r="B7" s="10">
         <v>1119</v>
       </c>
       <c r="C7">
         <v>802</v>
       </c>
-      <c r="E7" s="15">
+      <c r="E7" s="3">
         <v>45697</v>
       </c>
       <c r="F7">
@@ -1668,13 +1675,13 @@
       <c r="A8" s="3">
         <v>45704</v>
       </c>
-      <c r="B8" s="12">
+      <c r="B8" s="10">
         <v>1210</v>
       </c>
       <c r="C8">
         <v>794</v>
       </c>
-      <c r="E8" s="15">
+      <c r="E8" s="3">
         <v>45704</v>
       </c>
       <c r="F8">
@@ -1688,13 +1695,13 @@
       <c r="A9" s="3">
         <v>45711</v>
       </c>
-      <c r="B9" s="12">
+      <c r="B9" s="10">
         <v>1042</v>
       </c>
       <c r="C9">
         <v>703</v>
       </c>
-      <c r="E9" s="15">
+      <c r="E9" s="3">
         <v>45711</v>
       </c>
       <c r="F9">
@@ -1708,13 +1715,13 @@
       <c r="A10" s="3">
         <v>45718</v>
       </c>
-      <c r="B10" s="12">
+      <c r="B10" s="10">
         <v>1463</v>
       </c>
       <c r="C10">
         <v>986</v>
       </c>
-      <c r="E10" s="15">
+      <c r="E10" s="3">
         <v>45718</v>
       </c>
       <c r="F10">
@@ -1728,13 +1735,13 @@
       <c r="A11" s="3">
         <v>45725</v>
       </c>
-      <c r="B11" s="12">
+      <c r="B11" s="10">
         <v>1625</v>
       </c>
       <c r="C11">
         <v>864</v>
       </c>
-      <c r="E11" s="15">
+      <c r="E11" s="3">
         <v>45725</v>
       </c>
       <c r="F11">
@@ -1748,13 +1755,13 @@
       <c r="A12" s="3">
         <v>45732</v>
       </c>
-      <c r="B12" s="12">
+      <c r="B12" s="10">
         <v>1565</v>
       </c>
       <c r="C12">
         <v>781</v>
       </c>
-      <c r="E12" s="15">
+      <c r="E12" s="3">
         <v>45732</v>
       </c>
       <c r="F12">
@@ -1768,13 +1775,13 @@
       <c r="A13" s="3">
         <v>45739</v>
       </c>
-      <c r="B13" s="12">
+      <c r="B13" s="10">
         <v>1307</v>
       </c>
       <c r="C13">
         <v>1010</v>
       </c>
-      <c r="E13" s="15">
+      <c r="E13" s="3">
         <v>45739</v>
       </c>
       <c r="F13">
@@ -1788,13 +1795,13 @@
       <c r="A14" s="3">
         <v>45746</v>
       </c>
-      <c r="B14" s="12">
+      <c r="B14" s="10">
         <v>1191</v>
       </c>
       <c r="C14">
         <v>901</v>
       </c>
-      <c r="E14" s="15">
+      <c r="E14" s="3">
         <v>45746</v>
       </c>
       <c r="F14">
@@ -1808,13 +1815,13 @@
       <c r="A15" s="3">
         <v>45753</v>
       </c>
-      <c r="B15" s="12">
+      <c r="B15" s="10">
         <v>983</v>
       </c>
       <c r="C15">
         <v>875</v>
       </c>
-      <c r="E15" s="15">
+      <c r="E15" s="3">
         <v>45753</v>
       </c>
       <c r="F15">
@@ -1828,13 +1835,13 @@
       <c r="A16" s="3">
         <v>45760</v>
       </c>
-      <c r="B16" s="12">
+      <c r="B16" s="10">
         <v>1366</v>
       </c>
       <c r="C16">
         <v>845</v>
       </c>
-      <c r="E16" s="15">
+      <c r="E16" s="3">
         <v>45760</v>
       </c>
       <c r="F16">
@@ -1848,13 +1855,13 @@
       <c r="A17" s="3">
         <v>45767</v>
       </c>
-      <c r="B17" s="12">
+      <c r="B17" s="10">
         <v>1118</v>
       </c>
       <c r="C17">
         <v>728</v>
       </c>
-      <c r="E17" s="15">
+      <c r="E17" s="3">
         <v>45767</v>
       </c>
       <c r="F17">
@@ -1868,13 +1875,13 @@
       <c r="A18" s="3">
         <v>45774</v>
       </c>
-      <c r="B18" s="12">
+      <c r="B18" s="10">
         <v>1290</v>
       </c>
       <c r="C18">
         <v>1036</v>
       </c>
-      <c r="E18" s="15">
+      <c r="E18" s="3">
         <v>45774</v>
       </c>
       <c r="F18">
@@ -1888,13 +1895,13 @@
       <c r="A19" s="3">
         <v>45781</v>
       </c>
-      <c r="B19" s="12">
+      <c r="B19" s="10">
         <v>1314</v>
       </c>
       <c r="C19">
         <v>951</v>
       </c>
-      <c r="E19" s="15">
+      <c r="E19" s="3">
         <v>45781</v>
       </c>
       <c r="F19">
@@ -1908,13 +1915,13 @@
       <c r="A20" s="3">
         <v>45788</v>
       </c>
-      <c r="B20" s="12">
+      <c r="B20" s="10">
         <v>1492</v>
       </c>
       <c r="C20">
         <v>939</v>
       </c>
-      <c r="E20" s="15">
+      <c r="E20" s="3">
         <v>45788</v>
       </c>
       <c r="F20">
@@ -1928,13 +1935,13 @@
       <c r="A21" s="3">
         <v>45795</v>
       </c>
-      <c r="B21" s="12">
+      <c r="B21" s="10">
         <v>1232</v>
       </c>
       <c r="C21">
         <v>897</v>
       </c>
-      <c r="E21" s="15">
+      <c r="E21" s="3">
         <v>45795</v>
       </c>
       <c r="F21">
@@ -1948,13 +1955,13 @@
       <c r="A22" s="3">
         <v>45802</v>
       </c>
-      <c r="B22" s="12">
+      <c r="B22" s="10">
         <v>1128</v>
       </c>
       <c r="C22">
         <v>885</v>
       </c>
-      <c r="E22" s="15">
+      <c r="E22" s="3">
         <v>45802</v>
       </c>
       <c r="F22">
@@ -1968,13 +1975,13 @@
       <c r="A23" s="3">
         <v>45809</v>
       </c>
-      <c r="B23" s="12">
+      <c r="B23" s="10">
         <v>941</v>
       </c>
       <c r="C23">
         <v>688</v>
       </c>
-      <c r="E23" s="15">
+      <c r="E23" s="3">
         <v>45809</v>
       </c>
       <c r="F23">
@@ -1988,13 +1995,13 @@
       <c r="A24" s="3">
         <v>45816</v>
       </c>
-      <c r="B24" s="12">
+      <c r="B24" s="10">
         <v>1315</v>
       </c>
       <c r="C24">
         <v>884</v>
       </c>
-      <c r="E24" s="15">
+      <c r="E24" s="3">
         <v>45816</v>
       </c>
       <c r="F24">
@@ -2008,13 +2015,13 @@
       <c r="A25" s="3">
         <v>45823</v>
       </c>
-      <c r="B25" s="12">
+      <c r="B25" s="10">
         <v>1120</v>
       </c>
       <c r="C25">
         <v>745</v>
       </c>
-      <c r="E25" s="15">
+      <c r="E25" s="3">
         <v>45823</v>
       </c>
       <c r="F25">
@@ -2028,13 +2035,13 @@
       <c r="A26" s="3">
         <v>45830</v>
       </c>
-      <c r="B26" s="12">
+      <c r="B26" s="10">
         <v>1085</v>
       </c>
       <c r="C26">
         <v>668</v>
       </c>
-      <c r="E26" s="15">
+      <c r="E26" s="3">
         <v>45830</v>
       </c>
       <c r="F26">
@@ -2048,13 +2055,13 @@
       <c r="A27" s="3">
         <v>45837</v>
       </c>
-      <c r="B27" s="12">
+      <c r="B27" s="10">
         <v>1202</v>
       </c>
       <c r="C27">
         <v>763</v>
       </c>
-      <c r="E27" s="15">
+      <c r="E27" s="3">
         <v>45837</v>
       </c>
       <c r="F27">
@@ -2068,13 +2075,13 @@
       <c r="A28" s="3">
         <v>45844</v>
       </c>
-      <c r="B28" s="12">
+      <c r="B28" s="10">
         <v>903</v>
       </c>
       <c r="C28">
         <v>497</v>
       </c>
-      <c r="E28" s="15">
+      <c r="E28" s="3">
         <v>45844</v>
       </c>
       <c r="F28">
@@ -2088,13 +2095,13 @@
       <c r="A29" s="3">
         <v>45851</v>
       </c>
-      <c r="B29" s="12">
+      <c r="B29" s="10">
         <v>931</v>
       </c>
       <c r="C29">
         <v>594</v>
       </c>
-      <c r="E29" s="15">
+      <c r="E29" s="3">
         <v>45851</v>
       </c>
       <c r="F29">
@@ -2108,13 +2115,13 @@
       <c r="A30" s="3">
         <v>45858</v>
       </c>
-      <c r="B30" s="12">
+      <c r="B30" s="10">
         <v>1106</v>
       </c>
       <c r="C30">
         <v>693</v>
       </c>
-      <c r="E30" s="15">
+      <c r="E30" s="3">
         <v>45858</v>
       </c>
       <c r="F30">
@@ -2128,13 +2135,13 @@
       <c r="A31" s="3">
         <v>45865</v>
       </c>
-      <c r="B31" s="12">
+      <c r="B31" s="10">
         <v>1005</v>
       </c>
       <c r="C31">
         <v>651</v>
       </c>
-      <c r="E31" s="15">
+      <c r="E31" s="3">
         <v>45865</v>
       </c>
       <c r="F31">
@@ -2148,13 +2155,13 @@
       <c r="A32" s="3">
         <v>45872</v>
       </c>
-      <c r="B32" s="12">
+      <c r="B32" s="10">
         <v>1021</v>
       </c>
       <c r="C32">
         <v>633</v>
       </c>
-      <c r="E32" s="15">
+      <c r="E32" s="3">
         <v>45872</v>
       </c>
       <c r="F32">
@@ -2168,13 +2175,13 @@
       <c r="A33" s="3">
         <v>45879</v>
       </c>
-      <c r="B33" s="12">
+      <c r="B33" s="10">
         <v>1005</v>
       </c>
       <c r="C33">
         <v>839</v>
       </c>
-      <c r="E33" s="15">
+      <c r="E33" s="3">
         <v>45879</v>
       </c>
       <c r="F33">
@@ -2188,13 +2195,13 @@
       <c r="A34" s="3">
         <v>45886</v>
       </c>
-      <c r="B34" s="12">
+      <c r="B34" s="10">
         <v>1233</v>
       </c>
       <c r="C34">
         <v>978</v>
       </c>
-      <c r="E34" s="15">
+      <c r="E34" s="3">
         <v>45886</v>
       </c>
       <c r="F34">
@@ -2208,13 +2215,13 @@
       <c r="A35" s="3">
         <v>45893</v>
       </c>
-      <c r="B35" s="12">
+      <c r="B35" s="10">
         <v>1519</v>
       </c>
       <c r="C35">
         <v>800</v>
       </c>
-      <c r="E35" s="15">
+      <c r="E35" s="3">
         <v>45893</v>
       </c>
       <c r="F35">
@@ -2228,13 +2235,13 @@
       <c r="A36" s="3">
         <v>45900</v>
       </c>
-      <c r="B36" s="12">
+      <c r="B36" s="10">
         <v>1277</v>
       </c>
       <c r="C36">
         <v>756</v>
       </c>
-      <c r="E36" s="15">
+      <c r="E36" s="3">
         <v>45900</v>
       </c>
       <c r="F36">
@@ -2248,13 +2255,13 @@
       <c r="A37" s="3">
         <v>45907</v>
       </c>
-      <c r="B37" s="12">
+      <c r="B37" s="10">
         <v>1110</v>
       </c>
       <c r="C37">
         <v>896</v>
       </c>
-      <c r="E37" s="15">
+      <c r="E37" s="3">
         <v>45907</v>
       </c>
       <c r="F37">
@@ -2268,13 +2275,13 @@
       <c r="A38" s="3">
         <v>45914</v>
       </c>
-      <c r="B38" s="12">
+      <c r="B38" s="10">
         <v>1731</v>
       </c>
       <c r="C38">
         <v>1039</v>
       </c>
-      <c r="E38" s="15">
+      <c r="E38" s="3">
         <v>45914</v>
       </c>
       <c r="F38">
@@ -2288,13 +2295,13 @@
       <c r="A39" s="3">
         <v>45921</v>
       </c>
-      <c r="B39" s="12">
+      <c r="B39" s="10">
         <v>1271</v>
       </c>
       <c r="C39">
         <v>1221</v>
       </c>
-      <c r="E39" s="15">
+      <c r="E39" s="3">
         <v>45921</v>
       </c>
       <c r="F39">
@@ -2308,13 +2315,13 @@
       <c r="A40" s="3">
         <v>45928</v>
       </c>
-      <c r="B40" s="12">
+      <c r="B40" s="10">
         <v>1373</v>
       </c>
       <c r="C40">
         <v>925</v>
       </c>
-      <c r="E40" s="15">
+      <c r="E40" s="3">
         <v>45928</v>
       </c>
       <c r="F40">
@@ -2328,13 +2335,13 @@
       <c r="A41" s="3">
         <v>45935</v>
       </c>
-      <c r="B41" s="12">
+      <c r="B41" s="10">
         <v>1263</v>
       </c>
       <c r="C41">
         <v>969</v>
       </c>
-      <c r="E41" s="15">
+      <c r="E41" s="3">
         <v>45935</v>
       </c>
       <c r="F41">
@@ -2348,13 +2355,13 @@
       <c r="A42" s="3">
         <v>45942</v>
       </c>
-      <c r="B42" s="12">
+      <c r="B42" s="10">
         <v>1239</v>
       </c>
       <c r="C42">
         <v>927</v>
       </c>
-      <c r="E42" s="15">
+      <c r="E42" s="3">
         <v>45942</v>
       </c>
       <c r="F42">
@@ -2368,13 +2375,13 @@
       <c r="A43" s="3">
         <v>45949</v>
       </c>
-      <c r="B43" s="13">
+      <c r="B43" s="11">
         <v>1394</v>
       </c>
       <c r="C43">
         <v>1140</v>
       </c>
-      <c r="E43" s="15">
+      <c r="E43" s="3">
         <v>45949</v>
       </c>
       <c r="F43">
@@ -2388,13 +2395,13 @@
       <c r="A44" s="3">
         <v>45956</v>
       </c>
-      <c r="B44" s="12">
+      <c r="B44" s="10">
         <v>1504</v>
       </c>
       <c r="C44">
         <v>913</v>
       </c>
-      <c r="E44" s="15">
+      <c r="E44" s="3">
         <v>45956</v>
       </c>
       <c r="F44">
@@ -2408,24 +2415,30 @@
       <c r="A45" s="3">
         <v>45963</v>
       </c>
-      <c r="B45" s="12">
+      <c r="B45" s="10">
         <v>1398</v>
       </c>
-      <c r="E45" s="15">
+      <c r="C45">
+        <v>946</v>
+      </c>
+      <c r="E45" s="3">
         <v>45963</v>
       </c>
       <c r="F45">
         <v>0.92090000000000005</v>
+      </c>
+      <c r="G45">
+        <v>0.96930000000000005</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="15.75">
       <c r="A46" s="3">
         <v>45970</v>
       </c>
-      <c r="B46" s="12">
+      <c r="B46" s="10">
         <v>1397</v>
       </c>
-      <c r="E46" s="15">
+      <c r="E46" s="3">
         <v>45970</v>
       </c>
       <c r="F46">
@@ -2436,10 +2449,10 @@
       <c r="A47" s="3">
         <v>45977</v>
       </c>
-      <c r="B47" s="12">
+      <c r="B47" s="10">
         <v>1241</v>
       </c>
-      <c r="E47" s="15">
+      <c r="E47" s="3">
         <v>45977</v>
       </c>
       <c r="F47">
@@ -2450,10 +2463,10 @@
       <c r="A48" s="3">
         <v>45984</v>
       </c>
-      <c r="B48" s="12">
+      <c r="B48" s="10">
         <v>1950</v>
       </c>
-      <c r="E48" s="15">
+      <c r="E48" s="3">
         <v>45984</v>
       </c>
       <c r="F48">
@@ -2464,10 +2477,10 @@
       <c r="A49" s="3">
         <v>45991</v>
       </c>
-      <c r="B49" s="14">
+      <c r="B49" s="12">
         <v>799</v>
       </c>
-      <c r="E49" s="15">
+      <c r="E49" s="3">
         <v>45991</v>
       </c>
       <c r="F49">
@@ -2478,10 +2491,10 @@
       <c r="A50" s="3">
         <v>45998</v>
       </c>
-      <c r="B50" s="14">
+      <c r="B50" s="12">
         <v>1628</v>
       </c>
-      <c r="E50" s="15">
+      <c r="E50" s="3">
         <v>45998</v>
       </c>
       <c r="F50">
@@ -2492,10 +2505,10 @@
       <c r="A51" s="3">
         <v>46005</v>
       </c>
-      <c r="B51" s="14">
+      <c r="B51" s="12">
         <v>1566</v>
       </c>
-      <c r="E51" s="15">
+      <c r="E51" s="3">
         <v>46005</v>
       </c>
       <c r="F51">
@@ -2506,10 +2519,10 @@
       <c r="A52" s="3">
         <v>46012</v>
       </c>
-      <c r="B52" s="12">
+      <c r="B52" s="10">
         <v>918</v>
       </c>
-      <c r="E52" s="15">
+      <c r="E52" s="3">
         <v>46012</v>
       </c>
       <c r="F52">
@@ -2520,10 +2533,10 @@
       <c r="A53" s="3">
         <v>46019</v>
       </c>
-      <c r="B53" s="12">
+      <c r="B53" s="10">
         <v>450</v>
       </c>
-      <c r="E53" s="15">
+      <c r="E53" s="3">
         <v>46019</v>
       </c>
     </row>

</xml_diff>